<commit_message>
Fixed bug that prevents user from entering null string when clicking into the export to excel button
</commit_message>
<xml_diff>
--- a/LeapLog/bin/Debug/netcoreapp3.1/tableOne.xlsx
+++ b/LeapLog/bin/Debug/netcoreapp3.1/tableOne.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/139cebc20cf1c155/01LoneStar/2020Spring/INEW2332Project/NewGithubClone/leaplog/LeapLog/bin/Debug/netcoreapp3.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0A24F9E-4612-4249-968B-6235C3D67DCB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A5A9C610-CC06-49A6-99EB-582C6BE4CAB9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2415" yWindow="3120" windowWidth="21600" windowHeight="12735" xr2:uid="{6C5A6BFF-1549-4C1B-838F-C20F6CD68BD1}"/>
+    <workbookView xWindow="3945" yWindow="2805" windowWidth="21600" windowHeight="12735" xr2:uid="{6B115A59-04D3-417F-9A1F-FC84089BFC31}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -511,7 +511,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{792B50E9-DB5E-4A18-BF91-E782B96BE32D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E1ADD96-4C40-4714-AA3F-FC7E53B93C0F}">
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Added Journal Entry name to sheet
</commit_message>
<xml_diff>
--- a/LeapLog/bin/Debug/netcoreapp3.1/tableOne.xlsx
+++ b/LeapLog/bin/Debug/netcoreapp3.1/tableOne.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/139cebc20cf1c155/01LoneStar/2020Spring/INEW2332Project/NewGithubClone/leaplog/LeapLog/bin/Debug/netcoreapp3.1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/139cebc20cf1c155/01LoneStar/2020Spring/INEW2332Project/NewGit/leaplog/LeapLog/bin/Debug/netcoreapp3.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{A5A9C610-CC06-49A6-99EB-582C6BE4CAB9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{227C08F9-FB9B-4780-90F7-51BEB748997E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{88E39884-AED5-400F-8546-D39F930D1B31}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3945" yWindow="2805" windowWidth="21600" windowHeight="12735" xr2:uid="{6B115A59-04D3-417F-9A1F-FC84089BFC31}"/>
+    <workbookView xWindow="2685" yWindow="4290" windowWidth="21600" windowHeight="12735" xr2:uid="{2F5E79D2-522C-4C56-9CFE-B07AEAE7A8BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -512,7 +511,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E1ADD96-4C40-4714-AA3F-FC7E53B93C0F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96D1ABB0-56CC-4EA7-8857-B193245ED4D2}">
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -819,16 +818,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3407070C-B745-4B03-98BF-D57A514F451B}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated excel exports all tables in One Excel file
</commit_message>
<xml_diff>
--- a/LeapLog/bin/Debug/netcoreapp3.1/tableOne.xlsx
+++ b/LeapLog/bin/Debug/netcoreapp3.1/tableOne.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/139cebc20cf1c155/01LoneStar/2020Spring/INEW2332Project/NewGithubClone/leaplog/LeapLog/bin/Debug/netcoreapp3.1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/139cebc20cf1c155/01LoneStar/2020Spring/INEW2332Project/NewGit/leaplog/LeapLog/bin/Debug/netcoreapp3.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{A5A9C610-CC06-49A6-99EB-582C6BE4CAB9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{227C08F9-FB9B-4780-90F7-51BEB748997E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4C3B44E-1B0B-4DCC-A991-0114497C1231}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3945" yWindow="2805" windowWidth="21600" windowHeight="12735" xr2:uid="{6B115A59-04D3-417F-9A1F-FC84089BFC31}"/>
+    <workbookView xWindow="-25560" yWindow="1275" windowWidth="21600" windowHeight="12735" activeTab="4" xr2:uid="{BD82CDBA-7651-4562-9898-6955A4336220}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Statement of Owner Equity" sheetId="5" r:id="rId1"/>
+    <sheet name="Income Statement" sheetId="4" r:id="rId2"/>
+    <sheet name="Balance Sheet" sheetId="3" r:id="rId3"/>
+    <sheet name="T Accounts" sheetId="2" r:id="rId4"/>
+    <sheet name="Journal" sheetId="1" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="31">
   <si>
     <t>ID</t>
   </si>
@@ -56,6 +59,9 @@
   </si>
   <si>
     <t>Credit</t>
+  </si>
+  <si>
+    <t>FILL IN</t>
   </si>
   <si>
     <t>Bank of America</t>
@@ -512,7 +518,103 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E1ADD96-4C40-4714-AA3F-FC7E53B93C0F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38569739-0F9A-4716-8254-E18A61EBB27F}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49BBF1B2-9D87-4380-9ECF-C0B6ED51BF75}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28A6F260-50C3-4358-B47C-DFCEBC81D73B}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C6AE502-754A-45F2-A6AE-A514A2A4C985}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62D54B3E-8158-4F00-A38D-C6DD3CD6A1B9}">
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -563,19 +665,19 @@
         <v>43945</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1">
         <v>1200</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H2" s="1">
         <v>1200</v>
@@ -589,19 +691,19 @@
         <v>43945</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1">
         <v>5000</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H3" s="1">
         <v>5000</v>
@@ -615,19 +717,19 @@
         <v>43945</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1">
         <v>500</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H4" s="1">
         <v>500</v>
@@ -641,19 +743,19 @@
         <v>43945</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1">
         <v>700</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H5" s="1">
         <v>700</v>
@@ -667,19 +769,19 @@
         <v>43945</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E6" s="1">
         <v>900</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H6" s="1">
         <v>900</v>
@@ -693,19 +795,19 @@
         <v>43945</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E7" s="1">
         <v>600</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H7" s="1">
         <v>600</v>
@@ -719,19 +821,19 @@
         <v>43945</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E8" s="1">
         <v>400</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H8" s="1">
         <v>400</v>
@@ -745,19 +847,19 @@
         <v>43945</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E9" s="1">
         <v>400</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H9" s="1">
         <v>400</v>
@@ -771,19 +873,19 @@
         <v>43945</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E10" s="1">
         <v>4000</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H10" s="1">
         <v>4000</v>
@@ -797,19 +899,19 @@
         <v>43945</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E11" s="3">
         <v>6450</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H11" s="3">
         <v>6450</v>
@@ -819,16 +921,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3407070C-B745-4B03-98BF-D57A514F451B}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>